<commit_message>
Active and reactive power bal
Added active and reactive power balance in code.
</commit_message>
<xml_diff>
--- a/Data_3bus.xlsx
+++ b/Data_3bus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hakonsol\PycharmProjects\First_Project\OPF_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01A740D-E29D-490B-9CF3-2291592B1B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4A6C73-2C98-4A0E-8752-3C28A53293E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{12F1BD29-A7C3-4016-A696-A3E3AF7A56D0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{12F1BD29-A7C3-4016-A696-A3E3AF7A56D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Node data" sheetId="3" r:id="rId1"/>
@@ -748,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C6C254-8727-469B-84A8-B23DD509C36A}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -939,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E222ED-9C46-4E77-9318-E5530826F65A}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>